<commit_message>
Coupon page methods and objects
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satheesh.c\eclipse-workspace\hungerrush.hub\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE14F9-2133-4EB2-92FF-2EA95C2FA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AA11AA-B9A8-436F-BCFD-D7D0D79685E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5883AB23-DA68-4932-898D-4DD566FC5870}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7360" xr2:uid="{5883AB23-DA68-4932-898D-4DD566FC5870}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGINDATA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>testcasename</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>addCoupon</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -442,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D41D5D3-D937-4F36-8221-5F026CD246A4}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,7 +485,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -496,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -513,7 +519,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -522,6 +528,23 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>